<commit_message>
Fixing string errors and others
</commit_message>
<xml_diff>
--- a/GameEngineBase/TODO.xlsx
+++ b/GameEngineBase/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>DirectX 11</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>DebugRenderer Present()</t>
+  </si>
+  <si>
+    <t>DX11Renderer STD::COUT Description</t>
+  </si>
+  <si>
+    <t>std::cout logging to defined function</t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,6 +725,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Edits to math library and camera classes
</commit_message>
<xml_diff>
--- a/GameEngineBase/TODO.xlsx
+++ b/GameEngineBase/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>DirectX 11</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Vulkan</t>
   </si>
   <si>
-    <t>BufferLayout.cpp m_Size</t>
-  </si>
-  <si>
     <t>Assertions</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
     <t>GLShader.cpp ResolveUniforms() Bracketing</t>
   </si>
   <si>
-    <t>BufferLayout - Vulkan</t>
-  </si>
-  <si>
-    <t>Context - Vulkan</t>
-  </si>
-  <si>
     <t>BufferLayout</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
   </si>
   <si>
     <t>DX11Shader ParseStruct() - type == ":"</t>
-  </si>
-  <si>
-    <t>DX11Shader ParseCBuffer() - FindStruct(type) not name?</t>
   </si>
   <si>
     <t>DX11Shader ParseSamplerState() - push_back(declaration)</t>
@@ -552,7 +540,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,19 +553,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,16 +573,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,13 +590,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,34 +604,31 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -652,92 +637,83 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Render API dependant object code updates
</commit_message>
<xml_diff>
--- a/GameEngineBase/TODO.xlsx
+++ b/GameEngineBase/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>DirectX 11</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Change model format to custom</t>
+  </si>
+  <si>
+    <t>Framebuffer RenderAPI Employment</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +713,9 @@
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="E14" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">

</xml_diff>

<commit_message>
Fully implemented log system
</commit_message>
<xml_diff>
--- a/GameEngineBase/TODO.xlsx
+++ b/GameEngineBase/TODO.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716CA76A-E5E0-4629-A676-768B2248D632}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +723,9 @@
         <v>43</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Window->Clear(), Window->Update() - Except Renderer::Present() optimizations
</commit_message>
<xml_diff>
--- a/GameEngineBase/TODO.xlsx
+++ b/GameEngineBase/TODO.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716CA76A-E5E0-4629-A676-768B2248D632}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE56854-0710-4045-B54D-1A482664BC45}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>DirectX 11</t>
   </si>
@@ -52,9 +52,6 @@
     <t>MAIN WORK</t>
   </si>
   <si>
-    <t>__debugbreak() with assertions</t>
-  </si>
-  <si>
     <t>GLTexture2D setData(uint color)</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
   </si>
   <si>
     <t>DX11Renderer STD::COUT Description</t>
-  </si>
-  <si>
-    <t>std::cout logging to defined function</t>
   </si>
   <si>
     <t>Change model format to custom</t>
@@ -544,7 +538,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,13 +571,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -597,10 +591,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -608,27 +602,27 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -636,7 +630,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,10 +638,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,71 +649,63 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>